<commit_message>
Changed colors in metrics chart
</commit_message>
<xml_diff>
--- a/Presentation/images/Metrics.xlsx
+++ b/Presentation/images/Metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BHS2020\bhs-proj\Presentation\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07992E65-AA1A-4054-A756-E7A267B78D23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E7A68E-C72D-45EC-A164-829B96993522}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{63D1C6CC-5EDA-43B5-950A-C532E18BE1FE}"/>
   </bookViews>
@@ -35,9 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>Classification Model</t>
-  </si>
-  <si>
     <t>Accuracy</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>Random Forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classification Model      Metrics  </t>
   </si>
 </sst>
 </file>
@@ -92,13 +92,13 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,24 +107,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="6" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -132,38 +138,39 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -180,6 +187,70 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1051560</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>541020</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82E69962-B814-428B-BB7C-B25886539CA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1844040" y="403860"/>
+          <a:ext cx="1036320" cy="502920"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -479,206 +550,353 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F15BDC-D417-4C67-8564-D8D6026B647B}">
-  <dimension ref="D3:K10"/>
+  <dimension ref="D3:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.88671875" customWidth="1"/>
-    <col min="7" max="7" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="0.77734375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="8.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:11" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="D3" s="4" t="s">
+    <row r="3" spans="4:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="G3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="H3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="I3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="J3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="K3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="L3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="3" t="s">
+    </row>
+    <row r="4" spans="4:12" s="1" customFormat="1" ht="5.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="4:12" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D5" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="4:11" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D4" s="4" t="s">
+      <c r="E5" s="4"/>
+      <c r="F5" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.61</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.51</v>
+      </c>
+      <c r="I5" s="2">
+        <v>25</v>
+      </c>
+      <c r="J5" s="2">
+        <v>24</v>
+      </c>
+      <c r="K5" s="2">
+        <v>38</v>
+      </c>
+      <c r="L5" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="4:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="9"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="4:12" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="2">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.61</v>
-      </c>
-      <c r="G4" s="2">
+      <c r="E7" s="4"/>
+      <c r="F7" s="2">
         <v>0.51</v>
       </c>
-      <c r="H4" s="2">
+      <c r="G7" s="2">
+        <v>0.49</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="I7" s="2">
+        <v>23</v>
+      </c>
+      <c r="J7" s="2">
+        <v>26</v>
+      </c>
+      <c r="K7" s="2">
+        <v>32</v>
+      </c>
+      <c r="L7" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="4:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="9"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="4:12" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="I9" s="2">
+        <v>20</v>
+      </c>
+      <c r="J9" s="2">
+        <v>29</v>
+      </c>
+      <c r="K9" s="2">
+        <v>45</v>
+      </c>
+      <c r="L9" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="4:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="9"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="4:12" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="I11" s="2">
+        <v>16</v>
+      </c>
+      <c r="J11" s="2">
+        <v>33</v>
+      </c>
+      <c r="K11" s="2">
+        <v>35</v>
+      </c>
+      <c r="L11" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="4:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="9"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="4:12" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.54</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="I13" s="2">
         <v>25</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J13" s="2">
         <v>24</v>
       </c>
-      <c r="J4" s="2">
-        <v>38</v>
-      </c>
-      <c r="K4" s="2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="4:11" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.51</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.49</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0.47</v>
-      </c>
-      <c r="H5" s="2">
-        <v>23</v>
-      </c>
-      <c r="I5" s="2">
-        <v>26</v>
-      </c>
-      <c r="J5" s="2">
-        <v>32</v>
-      </c>
-      <c r="K5" s="2">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="4:11" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.59</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0.47</v>
-      </c>
-      <c r="H6" s="2">
-        <v>20</v>
-      </c>
-      <c r="I6" s="2">
+      <c r="K13" s="2">
+        <v>30</v>
+      </c>
+      <c r="L13" s="2">
         <v>29</v>
       </c>
-      <c r="J6" s="2">
-        <v>45</v>
-      </c>
-      <c r="K6" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="4:11" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.47</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.48</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0.32</v>
-      </c>
-      <c r="H7" s="2">
+    </row>
+    <row r="14" spans="4:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="9"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="4:12" s="1" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="I15" s="2">
+        <v>18</v>
+      </c>
+      <c r="J15" s="2">
+        <v>31</v>
+      </c>
+      <c r="K15" s="2">
+        <v>43</v>
+      </c>
+      <c r="L15" s="2">
         <v>16</v>
       </c>
-      <c r="I7" s="2">
-        <v>33</v>
-      </c>
-      <c r="J7" s="2">
-        <v>35</v>
-      </c>
-      <c r="K7" s="2">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="4:11" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.54</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0.52</v>
-      </c>
-      <c r="H8" s="2">
-        <v>25</v>
-      </c>
-      <c r="I8" s="2">
-        <v>24</v>
-      </c>
-      <c r="J8" s="2">
-        <v>30</v>
-      </c>
-      <c r="K8" s="2">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="4:11" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.52</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0.35</v>
-      </c>
-      <c r="H9" s="2">
-        <v>18</v>
-      </c>
-      <c r="I9" s="2">
-        <v>31</v>
-      </c>
-      <c r="J9" s="2">
-        <v>43</v>
-      </c>
-      <c r="K9" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="4:11" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    </row>
+    <row r="16" spans="4:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="7"/>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="F5:F15">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:G15">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:H15">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5:I15">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5:J15">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5:K15">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L5:L15">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>